<commit_message>
Switched QuestUIs and PersonUIs from instantiation to object pools, implemented Menu superclass
</commit_message>
<xml_diff>
--- a/documentation/WorldLore.xlsx
+++ b/documentation/WorldLore.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User\Documents\Projects\Unity\Adventure Guild\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D98ABB27-E63F-4879-85CC-1EED3E96B186}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F04361F-E094-4C6D-A007-A71FA430CD74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B1B6881F-5ED0-440A-8634-A42A5146A78F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Location</t>
   </si>
@@ -136,6 +136,24 @@
   </si>
   <si>
     <t>Waylaid by ghouls</t>
+  </si>
+  <si>
+    <t>Village of Crast</t>
+  </si>
+  <si>
+    <t>South, beyond the river</t>
+  </si>
+  <si>
+    <t>Location Info</t>
+  </si>
+  <si>
+    <t>Attacked by a gryphon</t>
+  </si>
+  <si>
+    <t>Ealdorman Westnedge</t>
+  </si>
+  <si>
+    <t>15002 Torment of Talons</t>
   </si>
 </sst>
 </file>
@@ -200,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -228,6 +246,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,19 +564,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A73FE0-8F21-4723-B69E-6787F3A01C6B}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="30.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" style="5" customWidth="1"/>
+    <col min="1" max="3" width="30.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,14 +588,17 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -582,14 +608,14 @@
       <c r="C2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
@@ -599,12 +625,12 @@
       <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="10"/>
+      <c r="F3" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
@@ -614,78 +640,95 @@
       <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to Unity 2019.4.28f1, add a quest
</commit_message>
<xml_diff>
--- a/documentation/WorldLore.xlsx
+++ b/documentation/WorldLore.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User\Documents\Projects\Unity\Adventure Guild\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\Projects\Unity\AdventureGuild\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F04361F-E094-4C6D-A007-A71FA430CD74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AC63E3-EDB0-489D-8CC9-A1A1A56CA07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B1B6881F-5ED0-440A-8634-A42A5146A78F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B1B6881F-5ED0-440A-8634-A42A5146A78F}"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Location</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>15002 Torment of Talons</t>
+  </si>
+  <si>
+    <t>Town of Belmere</t>
+  </si>
+  <si>
+    <t>001012 Burden of Beast</t>
   </si>
 </sst>
 </file>
@@ -564,21 +570,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A73FE0-8F21-4723-B69E-6787F3A01C6B}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="30.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="5" customWidth="1"/>
+    <col min="1" max="3" width="30.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -598,7 +604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -615,7 +621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
@@ -630,7 +636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
@@ -647,7 +653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -658,7 +664,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -670,7 +676,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -681,7 +687,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -692,7 +698,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -703,7 +709,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -714,7 +720,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
@@ -729,6 +735,14 @@
       </c>
       <c r="F11" s="5" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ArtisanStats to the PersonUI, adjust passive recruitment frequency, add new quest chain
</commit_message>
<xml_diff>
--- a/documentation/WorldLore.xlsx
+++ b/documentation/WorldLore.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\Projects\Unity\AdventureGuild\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User\Documents\Projects\Unity\Adventure Guild\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AC63E3-EDB0-489D-8CC9-A1A1A56CA07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD62CF2-683E-41E3-8945-479797D68C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B1B6881F-5ED0-440A-8634-A42A5146A78F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{B1B6881F-5ED0-440A-8634-A42A5146A78F}"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Location</t>
   </si>
@@ -159,7 +159,14 @@
     <t>Town of Belmere</t>
   </si>
   <si>
-    <t>001012 Burden of Beast</t>
+    <t>Mayor Archenraed</t>
+  </si>
+  <si>
+    <t>001012 Burden of Beast
+001013 A Town in Trouble I
+005008 A Town in Trouble II
+010007 A Town in Trouble III
+015005 A Town in Trouble IV</t>
   </si>
 </sst>
 </file>
@@ -576,15 +583,15 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="30.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" style="5" customWidth="1"/>
+    <col min="1" max="3" width="30.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +611,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -621,7 +628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
@@ -636,7 +643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
@@ -653,7 +660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -664,7 +671,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -676,7 +683,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -687,7 +694,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -698,7 +705,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -709,7 +716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -720,7 +727,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
@@ -737,12 +744,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="2" t="s">
         <v>41</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the only level 20 quest
</commit_message>
<xml_diff>
--- a/documentation/WorldLore.xlsx
+++ b/documentation/WorldLore.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User\Documents\Projects\Unity\Adventure Guild\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD62CF2-683E-41E3-8945-479797D68C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B1209D-5DEC-478F-8F31-90FE157CB998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{B1B6881F-5ED0-440A-8634-A42A5146A78F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Location</t>
   </si>
@@ -167,6 +167,9 @@
 005008 A Town in Trouble II
 010007 A Town in Trouble III
 015005 A Town in Trouble IV</t>
+  </si>
+  <si>
+    <t>Kingdom of Calan</t>
   </si>
 </sst>
 </file>
@@ -231,36 +234,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -580,178 +577,181 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="30.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="5" customWidth="1"/>
+    <col min="1" max="3" width="30.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="4"/>
+      <c r="F3" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="2" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove HP from artisan and peasant PersonUIs, add a new quest
</commit_message>
<xml_diff>
--- a/documentation/WorldLore.xlsx
+++ b/documentation/WorldLore.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User\Documents\Projects\Unity\Adventure Guild\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B1209D-5DEC-478F-8F31-90FE157CB998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614332D8-AF23-4D94-8B33-70500FE16B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{B1B6881F-5ED0-440A-8634-A42A5146A78F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Location</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t>Kingdom of Calan</t>
+  </si>
+  <si>
+    <t>Port of Parilac</t>
+  </si>
+  <si>
+    <t>015006 The Perilous Port</t>
+  </si>
+  <si>
+    <t>Taken over by pirates</t>
   </si>
 </sst>
 </file>
@@ -574,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A73FE0-8F21-4723-B69E-6787F3A01C6B}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,6 +764,17 @@
         <v>42</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:E9">
     <sortCondition ref="A5:A9"/>

</xml_diff>